<commit_message>
debug dodecahedron creation a fix crash bugs
Subdivision is still buggy
</commit_message>
<xml_diff>
--- a/PlanetLibrary/TheoryWorkbook.xlsx
+++ b/PlanetLibrary/TheoryWorkbook.xlsx
@@ -17,7 +17,7 @@
   <definedNames>
     <definedName name="a">Sheet1!$B$5</definedName>
     <definedName name="h">Sheet1!$B$2</definedName>
-    <definedName name="ordScale">Sheet1!$H$4</definedName>
+    <definedName name="ordScale">Sheet1!$I$4</definedName>
     <definedName name="rad">Sheet1!$H$3</definedName>
     <definedName name="x">Sheet1!$B$3</definedName>
     <definedName name="z">Sheet1!$B$4</definedName>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="35">
   <si>
     <t>h=</t>
   </si>
@@ -128,6 +128,15 @@
   </si>
   <si>
     <t>calc r=</t>
+  </si>
+  <si>
+    <t>volume =</t>
+  </si>
+  <si>
+    <t>surface area=</t>
+  </si>
+  <si>
+    <t>Center:</t>
   </si>
 </sst>
 </file>
@@ -450,8 +459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AH34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" topLeftCell="L13" workbookViewId="0">
+      <selection activeCell="W33" sqref="W33:AA33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -505,10 +514,10 @@
         <f>1-(h^2)</f>
         <v>0.61803398874989479</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <f>rad/SQRT(3)</f>
         <v>0.72654252800536101</v>
       </c>
@@ -524,10 +533,10 @@
       <c r="C5" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <f>(2*D23)/20*SQRT(250+110*SQRT(5))</f>
         <v>1.0000000000000002</v>
       </c>
@@ -543,6 +552,21 @@
       <c r="C6" t="s">
         <v>23</v>
       </c>
+      <c r="H6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I6">
+        <f>(2*z*ordScale)^3 *(15*7*SQRT(5))/4</f>
+        <v>42.513268759627536</v>
+      </c>
+      <c r="J6">
+        <f>I6/12</f>
+        <v>3.5427723966356282</v>
+      </c>
+      <c r="K6">
+        <f>J6/5</f>
+        <v>0.70855447932712567</v>
+      </c>
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -555,6 +579,17 @@
       <c r="C7" t="s">
         <v>25</v>
       </c>
+      <c r="H7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I7">
+        <f>3*(2*z*ordScale)^2*SQRT(25+10*SQRT(5))</f>
+        <v>16.650873085546532</v>
+      </c>
+      <c r="J7">
+        <f>I7/12</f>
+        <v>1.3875727571288776</v>
+      </c>
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -1220,6 +1255,82 @@
       <c r="G17">
         <v>13</v>
       </c>
+      <c r="I17" t="s">
+        <v>34</v>
+      </c>
+      <c r="J17">
+        <f>AVERAGE(J12:J16)</f>
+        <v>0.8506508083520401</v>
+      </c>
+      <c r="K17">
+        <f t="shared" ref="K17:M17" si="16">AVERAGE(K12:K16)</f>
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="16"/>
+        <v>0.5257311121191337</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="16"/>
+        <v>0.89805595315917086</v>
+      </c>
+      <c r="P17" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q17">
+        <f>AVERAGE(Q12:Q16)</f>
+        <v>0</v>
+      </c>
+      <c r="R17">
+        <f t="shared" ref="R17" si="17">AVERAGE(R12:R16)</f>
+        <v>-0.5257311121191337</v>
+      </c>
+      <c r="S17">
+        <f t="shared" ref="S17" si="18">AVERAGE(S12:S16)</f>
+        <v>0.8506508083520401</v>
+      </c>
+      <c r="T17">
+        <f t="shared" ref="T17" si="19">AVERAGE(T12:T16)</f>
+        <v>0.89805595315917086</v>
+      </c>
+      <c r="W17" t="s">
+        <v>34</v>
+      </c>
+      <c r="X17">
+        <f>AVERAGE(X12:X16)</f>
+        <v>0.5257311121191337</v>
+      </c>
+      <c r="Y17">
+        <f t="shared" ref="Y17" si="20">AVERAGE(Y12:Y16)</f>
+        <v>-0.8506508083520401</v>
+      </c>
+      <c r="Z17">
+        <f t="shared" ref="Z17" si="21">AVERAGE(Z12:Z16)</f>
+        <v>0</v>
+      </c>
+      <c r="AA17">
+        <f t="shared" ref="AA17" si="22">AVERAGE(AA12:AA16)</f>
+        <v>0.89805595315917086</v>
+      </c>
+      <c r="AD17" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE17">
+        <f>AVERAGE(AE12:AE16)</f>
+        <v>0</v>
+      </c>
+      <c r="AF17">
+        <f t="shared" ref="AF17" si="23">AVERAGE(AF12:AF16)</f>
+        <v>-0.5257311121191337</v>
+      </c>
+      <c r="AG17">
+        <f t="shared" ref="AG17" si="24">AVERAGE(AG12:AG16)</f>
+        <v>-0.8506508083520401</v>
+      </c>
+      <c r="AH17">
+        <f t="shared" ref="AH17" si="25">AVERAGE(AH12:AH16)</f>
+        <v>0.89805595315917086</v>
+      </c>
     </row>
     <row r="18" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A18">
@@ -1446,76 +1557,76 @@
         <v>12</v>
       </c>
       <c r="J21">
-        <f t="shared" ref="J21:J24" si="16">LOOKUP(I21,$A$12:$A$34,$B$12:$B$34)</f>
+        <f t="shared" ref="J21:J24" si="26">LOOKUP(I21,$A$12:$A$34,$B$12:$B$34)</f>
         <v>1.1755705045849465</v>
       </c>
       <c r="K21">
-        <f t="shared" ref="K21:K24" si="17">LOOKUP(I21,$A$12:$A$34,$C$12:$C$34)</f>
+        <f t="shared" ref="K21:K24" si="27">LOOKUP(I21,$A$12:$A$34,$C$12:$C$34)</f>
         <v>0.44902797657958543</v>
       </c>
       <c r="L21">
-        <f t="shared" ref="L21:L24" si="18">LOOKUP(I21,$A$12:$A$34,$D$12:$D$34)</f>
+        <f t="shared" ref="L21:L24" si="28">LOOKUP(I21,$A$12:$A$34,$D$12:$D$34)</f>
         <v>0</v>
       </c>
       <c r="M21">
-        <f t="shared" ref="M21:M23" si="19">SQRT((J21-J22)^2+(K21-K22)^2+(L21-L22)^2)</f>
+        <f t="shared" ref="M21:M23" si="29">SQRT((J21-J22)^2+(K21-K22)^2+(L21-L22)^2)</f>
         <v>0.89805595315917086</v>
       </c>
       <c r="P21">
         <v>14</v>
       </c>
       <c r="Q21">
-        <f t="shared" ref="Q21:Q24" si="20">LOOKUP(P21,$A$12:$A$34,$B$12:$B$34)</f>
+        <f t="shared" ref="Q21:Q24" si="30">LOOKUP(P21,$A$12:$A$34,$B$12:$B$34)</f>
         <v>-1.1755705045849465</v>
       </c>
       <c r="R21">
-        <f t="shared" ref="R21:R24" si="21">LOOKUP(P21,$A$12:$A$34,$C$12:$C$34)</f>
+        <f t="shared" ref="R21:R24" si="31">LOOKUP(P21,$A$12:$A$34,$C$12:$C$34)</f>
         <v>0.44902797657958543</v>
       </c>
       <c r="S21">
-        <f t="shared" ref="S21:S24" si="22">LOOKUP(P21,$A$12:$A$34,$D$12:$D$34)</f>
+        <f t="shared" ref="S21:S24" si="32">LOOKUP(P21,$A$12:$A$34,$D$12:$D$34)</f>
         <v>0</v>
       </c>
       <c r="T21">
-        <f t="shared" ref="T21:T23" si="23">SQRT((Q21-Q22)^2+(R21-R22)^2+(S21-S22)^2)</f>
+        <f t="shared" ref="T21:T23" si="33">SQRT((Q21-Q22)^2+(R21-R22)^2+(S21-S22)^2)</f>
         <v>0.89805595315917097</v>
       </c>
       <c r="W21">
         <v>11</v>
       </c>
       <c r="X21">
-        <f t="shared" ref="X21:X24" si="24">LOOKUP(W21,$A$12:$A$34,$B$12:$B$34)</f>
+        <f t="shared" ref="X21:X24" si="34">LOOKUP(W21,$A$12:$A$34,$B$12:$B$34)</f>
         <v>0</v>
       </c>
       <c r="Y21">
-        <f t="shared" ref="Y21:Y24" si="25">LOOKUP(W21,$A$12:$A$34,$C$12:$C$34)</f>
+        <f t="shared" ref="Y21:Y24" si="35">LOOKUP(W21,$A$12:$A$34,$C$12:$C$34)</f>
         <v>-1.1755705045849465</v>
       </c>
       <c r="Z21">
-        <f t="shared" ref="Z21:Z24" si="26">LOOKUP(W21,$A$12:$A$34,$D$12:$D$34)</f>
+        <f t="shared" ref="Z21:Z24" si="36">LOOKUP(W21,$A$12:$A$34,$D$12:$D$34)</f>
         <v>-0.44902797657958543</v>
       </c>
       <c r="AA21">
-        <f t="shared" ref="AA21:AA23" si="27">SQRT((X21-X22)^2+(Y21-Y22)^2+(Z21-Z22)^2)</f>
+        <f t="shared" ref="AA21:AA23" si="37">SQRT((X21-X22)^2+(Y21-Y22)^2+(Z21-Z22)^2)</f>
         <v>0.89805595315917086</v>
       </c>
       <c r="AD21">
         <v>19</v>
       </c>
       <c r="AE21">
-        <f t="shared" ref="AE21:AE24" si="28">LOOKUP(AD21,$A$12:$A$34,$B$12:$B$34)</f>
+        <f t="shared" ref="AE21:AE24" si="38">LOOKUP(AD21,$A$12:$A$34,$B$12:$B$34)</f>
         <v>-0.44902797657958543</v>
       </c>
       <c r="AF21">
-        <f t="shared" ref="AF21:AF24" si="29">LOOKUP(AD21,$A$12:$A$34,$C$12:$C$34)</f>
+        <f t="shared" ref="AF21:AF24" si="39">LOOKUP(AD21,$A$12:$A$34,$C$12:$C$34)</f>
         <v>0</v>
       </c>
       <c r="AG21">
-        <f t="shared" ref="AG21:AG24" si="30">LOOKUP(AD21,$A$12:$A$34,$D$12:$D$34)</f>
+        <f t="shared" ref="AG21:AG24" si="40">LOOKUP(AD21,$A$12:$A$34,$D$12:$D$34)</f>
         <v>-1.1755705045849465</v>
       </c>
       <c r="AH21">
-        <f t="shared" ref="AH21:AH23" si="31">SQRT((AE21-AE22)^2+(AF21-AF22)^2+(AG21-AG22)^2)</f>
+        <f t="shared" ref="AH21:AH23" si="41">SQRT((AE21-AE22)^2+(AF21-AF22)^2+(AG21-AG22)^2)</f>
         <v>0.89805595315917086</v>
       </c>
     </row>
@@ -1542,76 +1653,76 @@
         <v>13</v>
       </c>
       <c r="J22">
-        <f t="shared" si="16"/>
+        <f t="shared" si="26"/>
         <v>1.1755705045849465</v>
       </c>
       <c r="K22">
-        <f t="shared" si="17"/>
+        <f t="shared" si="27"/>
         <v>-0.44902797657958543</v>
       </c>
       <c r="L22">
-        <f t="shared" si="18"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="M22">
-        <f t="shared" si="19"/>
+        <f t="shared" si="29"/>
         <v>0.89805595315917097</v>
       </c>
       <c r="P22">
         <v>4</v>
       </c>
       <c r="Q22">
-        <f t="shared" si="20"/>
+        <f t="shared" si="30"/>
         <v>-0.72654252800536101</v>
       </c>
       <c r="R22">
-        <f t="shared" si="21"/>
+        <f t="shared" si="31"/>
         <v>0.72654252800536101</v>
       </c>
       <c r="S22">
-        <f t="shared" si="22"/>
+        <f t="shared" si="32"/>
         <v>0.72654252800536101</v>
       </c>
       <c r="T22">
-        <f t="shared" si="23"/>
+        <f t="shared" si="33"/>
         <v>0.89805595315917086</v>
       </c>
       <c r="W22">
         <v>10</v>
       </c>
       <c r="X22">
-        <f t="shared" si="24"/>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="Y22">
-        <f t="shared" si="25"/>
+        <f t="shared" si="35"/>
         <v>-1.1755705045849465</v>
       </c>
       <c r="Z22">
-        <f t="shared" si="26"/>
+        <f t="shared" si="36"/>
         <v>0.44902797657958543</v>
       </c>
       <c r="AA22">
-        <f t="shared" si="27"/>
+        <f t="shared" si="37"/>
         <v>0.89805595315917086</v>
       </c>
       <c r="AD22">
         <v>7</v>
       </c>
       <c r="AE22">
-        <f t="shared" si="28"/>
+        <f t="shared" si="38"/>
         <v>-0.72654252800536101</v>
       </c>
       <c r="AF22">
-        <f t="shared" si="29"/>
+        <f t="shared" si="39"/>
         <v>-0.72654252800536101</v>
       </c>
       <c r="AG22">
-        <f t="shared" si="30"/>
+        <f t="shared" si="40"/>
         <v>-0.72654252800536101</v>
       </c>
       <c r="AH22">
-        <f t="shared" si="31"/>
+        <f t="shared" si="41"/>
         <v>0.89805595315917097</v>
       </c>
     </row>
@@ -1643,76 +1754,76 @@
         <v>3</v>
       </c>
       <c r="J23">
-        <f t="shared" si="16"/>
+        <f t="shared" si="26"/>
         <v>0.72654252800536101</v>
       </c>
       <c r="K23">
-        <f t="shared" si="17"/>
+        <f t="shared" si="27"/>
         <v>-0.72654252800536101</v>
       </c>
       <c r="L23">
-        <f t="shared" si="18"/>
+        <f t="shared" si="28"/>
         <v>-0.72654252800536101</v>
       </c>
       <c r="M23">
-        <f t="shared" si="19"/>
+        <f t="shared" si="29"/>
         <v>0.89805595315917086</v>
       </c>
       <c r="P23">
         <v>8</v>
       </c>
       <c r="Q23">
-        <f t="shared" si="20"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="R23">
-        <f t="shared" si="21"/>
+        <f t="shared" si="31"/>
         <v>1.1755705045849465</v>
       </c>
       <c r="S23">
-        <f t="shared" si="22"/>
+        <f t="shared" si="32"/>
         <v>0.44902797657958543</v>
       </c>
       <c r="T23">
-        <f t="shared" si="23"/>
+        <f t="shared" si="33"/>
         <v>0.89805595315917086</v>
       </c>
       <c r="W23">
         <v>6</v>
       </c>
       <c r="X23">
-        <f t="shared" si="24"/>
+        <f t="shared" si="34"/>
         <v>-0.72654252800536101</v>
       </c>
       <c r="Y23">
-        <f t="shared" si="25"/>
+        <f t="shared" si="35"/>
         <v>-0.72654252800536101</v>
       </c>
       <c r="Z23">
-        <f t="shared" si="26"/>
+        <f t="shared" si="36"/>
         <v>0.72654252800536101</v>
       </c>
       <c r="AA23">
-        <f t="shared" si="27"/>
+        <f t="shared" si="37"/>
         <v>0.89805595315917097</v>
       </c>
       <c r="AD23">
         <v>15</v>
       </c>
       <c r="AE23">
-        <f t="shared" si="28"/>
+        <f t="shared" si="38"/>
         <v>-1.1755705045849465</v>
       </c>
       <c r="AF23">
-        <f t="shared" si="29"/>
+        <f t="shared" si="39"/>
         <v>-0.44902797657958543</v>
       </c>
       <c r="AG23">
-        <f t="shared" si="30"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="AH23">
-        <f t="shared" si="31"/>
+        <f t="shared" si="41"/>
         <v>0.89805595315917086</v>
       </c>
     </row>
@@ -1744,15 +1855,15 @@
         <v>18</v>
       </c>
       <c r="J24">
-        <f t="shared" si="16"/>
+        <f t="shared" si="26"/>
         <v>0.44902797657958543</v>
       </c>
       <c r="K24">
-        <f t="shared" si="17"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="L24">
-        <f t="shared" si="18"/>
+        <f t="shared" si="28"/>
         <v>-1.1755705045849465</v>
       </c>
       <c r="M24">
@@ -1763,15 +1874,15 @@
         <v>9</v>
       </c>
       <c r="Q24">
-        <f t="shared" si="20"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="R24">
-        <f t="shared" si="21"/>
+        <f t="shared" si="31"/>
         <v>1.1755705045849465</v>
       </c>
       <c r="S24">
-        <f t="shared" si="22"/>
+        <f t="shared" si="32"/>
         <v>-0.44902797657958543</v>
       </c>
       <c r="T24">
@@ -1782,15 +1893,15 @@
         <v>15</v>
       </c>
       <c r="X24">
-        <f t="shared" si="24"/>
+        <f t="shared" si="34"/>
         <v>-1.1755705045849465</v>
       </c>
       <c r="Y24">
-        <f t="shared" si="25"/>
+        <f t="shared" si="35"/>
         <v>-0.44902797657958543</v>
       </c>
       <c r="Z24">
-        <f t="shared" si="26"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="AA24">
@@ -1801,15 +1912,15 @@
         <v>14</v>
       </c>
       <c r="AE24">
-        <f t="shared" si="28"/>
+        <f t="shared" si="38"/>
         <v>-1.1755705045849465</v>
       </c>
       <c r="AF24">
-        <f t="shared" si="29"/>
+        <f t="shared" si="39"/>
         <v>0.44902797657958543</v>
       </c>
       <c r="AG24">
-        <f t="shared" si="30"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="AH24">
@@ -1841,6 +1952,82 @@
       <c r="G25">
         <v>6</v>
       </c>
+      <c r="I25" t="s">
+        <v>34</v>
+      </c>
+      <c r="J25">
+        <f>AVERAGE(J20:J24)</f>
+        <v>0.8506508083520401</v>
+      </c>
+      <c r="K25">
+        <f t="shared" ref="K25" si="42">AVERAGE(K20:K24)</f>
+        <v>0</v>
+      </c>
+      <c r="L25">
+        <f t="shared" ref="L25" si="43">AVERAGE(L20:L24)</f>
+        <v>-0.5257311121191337</v>
+      </c>
+      <c r="M25">
+        <f t="shared" ref="M25" si="44">AVERAGE(M20:M24)</f>
+        <v>0.89805595315917086</v>
+      </c>
+      <c r="P25" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q25">
+        <f>AVERAGE(Q20:Q24)</f>
+        <v>-0.5257311121191337</v>
+      </c>
+      <c r="R25">
+        <f t="shared" ref="R25" si="45">AVERAGE(R20:R24)</f>
+        <v>0.8506508083520401</v>
+      </c>
+      <c r="S25">
+        <f t="shared" ref="S25" si="46">AVERAGE(S20:S24)</f>
+        <v>0</v>
+      </c>
+      <c r="T25">
+        <f t="shared" ref="T25" si="47">AVERAGE(T20:T24)</f>
+        <v>0.89805595315917086</v>
+      </c>
+      <c r="W25" t="s">
+        <v>34</v>
+      </c>
+      <c r="X25">
+        <f>AVERAGE(X20:X24)</f>
+        <v>-0.5257311121191337</v>
+      </c>
+      <c r="Y25">
+        <f t="shared" ref="Y25" si="48">AVERAGE(Y20:Y24)</f>
+        <v>-0.8506508083520401</v>
+      </c>
+      <c r="Z25">
+        <f t="shared" ref="Z25" si="49">AVERAGE(Z20:Z24)</f>
+        <v>0</v>
+      </c>
+      <c r="AA25">
+        <f t="shared" ref="AA25" si="50">AVERAGE(AA20:AA24)</f>
+        <v>0.89805595315917086</v>
+      </c>
+      <c r="AD25" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE25">
+        <f>AVERAGE(AE20:AE24)</f>
+        <v>-0.8506508083520401</v>
+      </c>
+      <c r="AF25">
+        <f t="shared" ref="AF25" si="51">AVERAGE(AF20:AF24)</f>
+        <v>0</v>
+      </c>
+      <c r="AG25">
+        <f t="shared" ref="AG25" si="52">AVERAGE(AG20:AG24)</f>
+        <v>-0.5257311121191337</v>
+      </c>
+      <c r="AH25">
+        <f t="shared" ref="AH25" si="53">AVERAGE(AH20:AH24)</f>
+        <v>0.89805595315917086</v>
+      </c>
     </row>
     <row r="26" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A26">
@@ -2105,76 +2292,76 @@
         <v>8</v>
       </c>
       <c r="J29">
-        <f t="shared" ref="J29:J32" si="32">LOOKUP(I29,$A$12:$A$34,$B$12:$B$34)</f>
+        <f t="shared" ref="J29:J32" si="54">LOOKUP(I29,$A$12:$A$34,$B$12:$B$34)</f>
         <v>0</v>
       </c>
       <c r="K29">
-        <f t="shared" ref="K29:K32" si="33">LOOKUP(I29,$A$12:$A$34,$C$12:$C$34)</f>
+        <f t="shared" ref="K29:K32" si="55">LOOKUP(I29,$A$12:$A$34,$C$12:$C$34)</f>
         <v>1.1755705045849465</v>
       </c>
       <c r="L29">
-        <f t="shared" ref="L29:L32" si="34">LOOKUP(I29,$A$12:$A$34,$D$12:$D$34)</f>
+        <f t="shared" ref="L29:L32" si="56">LOOKUP(I29,$A$12:$A$34,$D$12:$D$34)</f>
         <v>0.44902797657958543</v>
       </c>
       <c r="M29">
-        <f t="shared" ref="M29:M31" si="35">SQRT((J29-J30)^2+(K29-K30)^2+(L29-L30)^2)</f>
+        <f t="shared" ref="M29:M31" si="57">SQRT((J29-J30)^2+(K29-K30)^2+(L29-L30)^2)</f>
         <v>0.89805595315917086</v>
       </c>
       <c r="P29">
         <v>9</v>
       </c>
       <c r="Q29">
-        <f t="shared" ref="Q29:Q32" si="36">LOOKUP(P29,$A$12:$A$34,$B$12:$B$34)</f>
+        <f t="shared" ref="Q29:Q32" si="58">LOOKUP(P29,$A$12:$A$34,$B$12:$B$34)</f>
         <v>0</v>
       </c>
       <c r="R29">
-        <f t="shared" ref="R29:R32" si="37">LOOKUP(P29,$A$12:$A$34,$C$12:$C$34)</f>
+        <f t="shared" ref="R29:R32" si="59">LOOKUP(P29,$A$12:$A$34,$C$12:$C$34)</f>
         <v>1.1755705045849465</v>
       </c>
       <c r="S29">
-        <f t="shared" ref="S29:S32" si="38">LOOKUP(P29,$A$12:$A$34,$D$12:$D$34)</f>
+        <f t="shared" ref="S29:S32" si="60">LOOKUP(P29,$A$12:$A$34,$D$12:$D$34)</f>
         <v>-0.44902797657958543</v>
       </c>
       <c r="T29">
-        <f t="shared" ref="T29:T31" si="39">SQRT((Q29-Q30)^2+(R29-R30)^2+(S29-S30)^2)</f>
+        <f t="shared" ref="T29:T31" si="61">SQRT((Q29-Q30)^2+(R29-R30)^2+(S29-S30)^2)</f>
         <v>0.89805595315917086</v>
       </c>
       <c r="W29">
         <v>9</v>
       </c>
       <c r="X29">
-        <f t="shared" ref="X29:X32" si="40">LOOKUP(W29,$A$12:$A$34,$B$12:$B$34)</f>
+        <f t="shared" ref="X29:X32" si="62">LOOKUP(W29,$A$12:$A$34,$B$12:$B$34)</f>
         <v>0</v>
       </c>
       <c r="Y29">
-        <f t="shared" ref="Y29:Y32" si="41">LOOKUP(W29,$A$12:$A$34,$C$12:$C$34)</f>
+        <f t="shared" ref="Y29:Y32" si="63">LOOKUP(W29,$A$12:$A$34,$C$12:$C$34)</f>
         <v>1.1755705045849465</v>
       </c>
       <c r="Z29">
-        <f t="shared" ref="Z29:Z32" si="42">LOOKUP(W29,$A$12:$A$34,$D$12:$D$34)</f>
+        <f t="shared" ref="Z29:Z32" si="64">LOOKUP(W29,$A$12:$A$34,$D$12:$D$34)</f>
         <v>-0.44902797657958543</v>
       </c>
       <c r="AA29">
-        <f t="shared" ref="AA29:AA31" si="43">SQRT((X29-X30)^2+(Y29-Y30)^2+(Z29-Z30)^2)</f>
+        <f t="shared" ref="AA29:AA31" si="65">SQRT((X29-X30)^2+(Y29-Y30)^2+(Z29-Z30)^2)</f>
         <v>0.89805595315917086</v>
       </c>
       <c r="AD29">
         <v>14</v>
       </c>
       <c r="AE29">
-        <f t="shared" ref="AE29:AE32" si="44">LOOKUP(AD29,$A$12:$A$34,$B$12:$B$34)</f>
+        <f t="shared" ref="AE29:AE32" si="66">LOOKUP(AD29,$A$12:$A$34,$B$12:$B$34)</f>
         <v>-1.1755705045849465</v>
       </c>
       <c r="AF29">
-        <f t="shared" ref="AF29:AF32" si="45">LOOKUP(AD29,$A$12:$A$34,$C$12:$C$34)</f>
+        <f t="shared" ref="AF29:AF32" si="67">LOOKUP(AD29,$A$12:$A$34,$C$12:$C$34)</f>
         <v>0.44902797657958543</v>
       </c>
       <c r="AG29">
-        <f t="shared" ref="AG29:AG32" si="46">LOOKUP(AD29,$A$12:$A$34,$D$12:$D$34)</f>
+        <f t="shared" ref="AG29:AG32" si="68">LOOKUP(AD29,$A$12:$A$34,$D$12:$D$34)</f>
         <v>0</v>
       </c>
       <c r="AH29">
-        <f t="shared" ref="AH29:AH31" si="47">SQRT((AE29-AE30)^2+(AF29-AF30)^2+(AG29-AG30)^2)</f>
+        <f t="shared" ref="AH29:AH31" si="69">SQRT((AE29-AE30)^2+(AF29-AF30)^2+(AG29-AG30)^2)</f>
         <v>0.89805595315917086</v>
       </c>
     </row>
@@ -2206,76 +2393,76 @@
         <v>4</v>
       </c>
       <c r="J30">
-        <f t="shared" si="32"/>
+        <f t="shared" si="54"/>
         <v>-0.72654252800536101</v>
       </c>
       <c r="K30">
-        <f t="shared" si="33"/>
+        <f t="shared" si="55"/>
         <v>0.72654252800536101</v>
       </c>
       <c r="L30">
-        <f t="shared" si="34"/>
+        <f t="shared" si="56"/>
         <v>0.72654252800536101</v>
       </c>
       <c r="M30">
-        <f t="shared" si="35"/>
+        <f t="shared" si="57"/>
         <v>0.89805595315917086</v>
       </c>
       <c r="P30">
         <v>8</v>
       </c>
       <c r="Q30">
-        <f t="shared" si="36"/>
+        <f t="shared" si="58"/>
         <v>0</v>
       </c>
       <c r="R30">
-        <f t="shared" si="37"/>
+        <f t="shared" si="59"/>
         <v>1.1755705045849465</v>
       </c>
       <c r="S30">
-        <f t="shared" si="38"/>
+        <f t="shared" si="60"/>
         <v>0.44902797657958543</v>
       </c>
       <c r="T30">
-        <f t="shared" si="39"/>
+        <f t="shared" si="61"/>
         <v>0.89805595315917086</v>
       </c>
       <c r="W30">
         <v>1</v>
       </c>
       <c r="X30">
-        <f t="shared" si="40"/>
+        <f t="shared" si="62"/>
         <v>0.72654252800536101</v>
       </c>
       <c r="Y30">
-        <f t="shared" si="41"/>
+        <f t="shared" si="63"/>
         <v>0.72654252800536101</v>
       </c>
       <c r="Z30">
-        <f t="shared" si="42"/>
+        <f t="shared" si="64"/>
         <v>-0.72654252800536101</v>
       </c>
       <c r="AA30">
-        <f t="shared" si="43"/>
+        <f t="shared" si="65"/>
         <v>0.89805595315917086</v>
       </c>
       <c r="AD30">
         <v>15</v>
       </c>
       <c r="AE30">
-        <f t="shared" si="44"/>
+        <f t="shared" si="66"/>
         <v>-1.1755705045849465</v>
       </c>
       <c r="AF30">
-        <f t="shared" si="45"/>
+        <f t="shared" si="67"/>
         <v>-0.44902797657958543</v>
       </c>
       <c r="AG30">
-        <f t="shared" si="46"/>
+        <f t="shared" si="68"/>
         <v>0</v>
       </c>
       <c r="AH30">
-        <f t="shared" si="47"/>
+        <f t="shared" si="69"/>
         <v>0.89805595315917097</v>
       </c>
     </row>
@@ -2307,76 +2494,76 @@
         <v>17</v>
       </c>
       <c r="J31">
-        <f t="shared" si="32"/>
+        <f t="shared" si="54"/>
         <v>-0.44902797657958543</v>
       </c>
       <c r="K31">
-        <f t="shared" si="33"/>
+        <f t="shared" si="55"/>
         <v>0</v>
       </c>
       <c r="L31">
-        <f t="shared" si="34"/>
+        <f t="shared" si="56"/>
         <v>1.1755705045849465</v>
       </c>
       <c r="M31">
-        <f t="shared" si="35"/>
+        <f t="shared" si="57"/>
         <v>0.89805595315917086</v>
       </c>
       <c r="P31">
         <v>0</v>
       </c>
       <c r="Q31">
-        <f t="shared" si="36"/>
+        <f t="shared" si="58"/>
         <v>0.72654252800536101</v>
       </c>
       <c r="R31">
-        <f t="shared" si="37"/>
+        <f t="shared" si="59"/>
         <v>0.72654252800536101</v>
       </c>
       <c r="S31">
-        <f t="shared" si="38"/>
+        <f t="shared" si="60"/>
         <v>0.72654252800536101</v>
       </c>
       <c r="T31">
-        <f t="shared" si="39"/>
+        <f t="shared" si="61"/>
         <v>0.89805595315917097</v>
       </c>
       <c r="W31">
         <v>18</v>
       </c>
       <c r="X31">
-        <f t="shared" si="40"/>
+        <f t="shared" si="62"/>
         <v>0.44902797657958543</v>
       </c>
       <c r="Y31">
-        <f t="shared" si="41"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="Z31">
-        <f t="shared" si="42"/>
+        <f t="shared" si="64"/>
         <v>-1.1755705045849465</v>
       </c>
       <c r="AA31">
-        <f t="shared" si="43"/>
+        <f t="shared" si="65"/>
         <v>0.89805595315917086</v>
       </c>
       <c r="AD31">
         <v>6</v>
       </c>
       <c r="AE31">
-        <f t="shared" si="44"/>
+        <f t="shared" si="66"/>
         <v>-0.72654252800536101</v>
       </c>
       <c r="AF31">
-        <f t="shared" si="45"/>
+        <f t="shared" si="67"/>
         <v>-0.72654252800536101</v>
       </c>
       <c r="AG31">
-        <f t="shared" si="46"/>
+        <f t="shared" si="68"/>
         <v>0.72654252800536101</v>
       </c>
       <c r="AH31">
-        <f t="shared" si="47"/>
+        <f t="shared" si="69"/>
         <v>0.89805595315917086</v>
       </c>
     </row>
@@ -2408,15 +2595,15 @@
         <v>16</v>
       </c>
       <c r="J32">
-        <f t="shared" si="32"/>
+        <f t="shared" si="54"/>
         <v>0.44902797657958543</v>
       </c>
       <c r="K32">
-        <f t="shared" si="33"/>
+        <f t="shared" si="55"/>
         <v>0</v>
       </c>
       <c r="L32">
-        <f t="shared" si="34"/>
+        <f t="shared" si="56"/>
         <v>1.1755705045849465</v>
       </c>
       <c r="M32">
@@ -2427,15 +2614,15 @@
         <v>12</v>
       </c>
       <c r="Q32">
-        <f t="shared" si="36"/>
+        <f t="shared" si="58"/>
         <v>1.1755705045849465</v>
       </c>
       <c r="R32">
-        <f t="shared" si="37"/>
+        <f t="shared" si="59"/>
         <v>0.44902797657958543</v>
       </c>
       <c r="S32">
-        <f t="shared" si="38"/>
+        <f t="shared" si="60"/>
         <v>0</v>
       </c>
       <c r="T32">
@@ -2446,15 +2633,15 @@
         <v>19</v>
       </c>
       <c r="X32">
-        <f t="shared" si="40"/>
+        <f t="shared" si="62"/>
         <v>-0.44902797657958543</v>
       </c>
       <c r="Y32">
-        <f t="shared" si="41"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="Z32">
-        <f t="shared" si="42"/>
+        <f t="shared" si="64"/>
         <v>-1.1755705045849465</v>
       </c>
       <c r="AA32">
@@ -2465,15 +2652,15 @@
         <v>17</v>
       </c>
       <c r="AE32">
-        <f t="shared" si="44"/>
+        <f t="shared" si="66"/>
         <v>-0.44902797657958543</v>
       </c>
       <c r="AF32">
-        <f t="shared" si="45"/>
+        <f t="shared" si="67"/>
         <v>0</v>
       </c>
       <c r="AG32">
-        <f t="shared" si="46"/>
+        <f t="shared" si="68"/>
         <v>1.1755705045849465</v>
       </c>
       <c r="AH32">
@@ -2481,7 +2668,7 @@
         <v>0.89805595315917086</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>18</v>
       </c>
@@ -2505,8 +2692,84 @@
       <c r="G33">
         <v>6</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I33" t="s">
+        <v>34</v>
+      </c>
+      <c r="J33">
+        <f>AVERAGE(J28:J32)</f>
+        <v>0</v>
+      </c>
+      <c r="K33">
+        <f t="shared" ref="K33" si="70">AVERAGE(K28:K32)</f>
+        <v>0.5257311121191337</v>
+      </c>
+      <c r="L33">
+        <f t="shared" ref="L33" si="71">AVERAGE(L28:L32)</f>
+        <v>0.8506508083520401</v>
+      </c>
+      <c r="M33">
+        <f t="shared" ref="M33" si="72">AVERAGE(M28:M32)</f>
+        <v>0.89805595315917086</v>
+      </c>
+      <c r="P33" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q33">
+        <f>AVERAGE(Q28:Q32)</f>
+        <v>0.5257311121191337</v>
+      </c>
+      <c r="R33">
+        <f t="shared" ref="R33" si="73">AVERAGE(R28:R32)</f>
+        <v>0.8506508083520401</v>
+      </c>
+      <c r="S33">
+        <f t="shared" ref="S33" si="74">AVERAGE(S28:S32)</f>
+        <v>0</v>
+      </c>
+      <c r="T33">
+        <f t="shared" ref="T33" si="75">AVERAGE(T28:T32)</f>
+        <v>0.89805595315917086</v>
+      </c>
+      <c r="W33" t="s">
+        <v>34</v>
+      </c>
+      <c r="X33">
+        <f>AVERAGE(X28:X32)</f>
+        <v>0</v>
+      </c>
+      <c r="Y33">
+        <f t="shared" ref="Y33" si="76">AVERAGE(Y28:Y32)</f>
+        <v>0.5257311121191337</v>
+      </c>
+      <c r="Z33">
+        <f t="shared" ref="Z33" si="77">AVERAGE(Z28:Z32)</f>
+        <v>-0.8506508083520401</v>
+      </c>
+      <c r="AA33">
+        <f t="shared" ref="AA33" si="78">AVERAGE(AA28:AA32)</f>
+        <v>0.89805595315917086</v>
+      </c>
+      <c r="AD33" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE33">
+        <f>AVERAGE(AE28:AE32)</f>
+        <v>-0.8506508083520401</v>
+      </c>
+      <c r="AF33">
+        <f t="shared" ref="AF33" si="79">AVERAGE(AF28:AF32)</f>
+        <v>0</v>
+      </c>
+      <c r="AG33">
+        <f t="shared" ref="AG33" si="80">AVERAGE(AG28:AG32)</f>
+        <v>0.5257311121191337</v>
+      </c>
+      <c r="AH33">
+        <f t="shared" ref="AH33" si="81">AVERAGE(AH28:AH32)</f>
+        <v>0.89805595315917086</v>
+      </c>
+    </row>
+    <row r="34" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>19</v>
       </c>

</xml_diff>